<commit_message>
merge branches to get base erin branch with all up to date changes in instream documentation
</commit_message>
<xml_diff>
--- a/data-raw/cottonwood_combined.xlsx
+++ b/data-raw/cottonwood_combined.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="19">
   <si>
     <t>Cottonwood creek downstream of south fork</t>
   </si>
@@ -69,6 +69,18 @@
   </si>
   <si>
     <t xml:space="preserve">length = 8.84 mi (CHECK) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Total length = 31.25 </t>
+  </si>
+  <si>
+    <t>non south fork total (for high flows) = 22.41</t>
+  </si>
+  <si>
+    <t>FR juv</t>
+  </si>
+  <si>
+    <t>ST juv</t>
   </si>
 </sst>
 </file>
@@ -386,23 +398,29 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:K48"/>
+  <dimension ref="A2:Q50"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="T16" sqref="T16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
       <c r="G2" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M2" t="s">
+        <v>15</v>
+      </c>
+      <c r="O2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -410,7 +428,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -441,8 +459,23 @@
       <c r="K4" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M4" t="s">
+        <v>2</v>
+      </c>
+      <c r="N4" t="s">
+        <v>17</v>
+      </c>
+      <c r="O4" t="s">
+        <v>9</v>
+      </c>
+      <c r="P4" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>15</v>
       </c>
@@ -464,8 +497,27 @@
       <c r="K5">
         <v>194136.29160063301</v>
       </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M5">
+        <v>15</v>
+      </c>
+      <c r="N5">
+        <f>(H5*(8.99/31.25)+H22*(13.42/31.25)+H39*(8.84/31.25))/5.28</f>
+        <v>50538.686419991282</v>
+      </c>
+      <c r="O5">
+        <f t="shared" ref="O5:Q17" si="0">(I5*(8.99/31.25)+I22*(13.42/31.25)+I39*(8.84/31.25))/5.28</f>
+        <v>160205.4550485611</v>
+      </c>
+      <c r="P5">
+        <f t="shared" si="0"/>
+        <v>11339.018044575716</v>
+      </c>
+      <c r="Q5">
+        <f t="shared" si="0"/>
+        <v>31631.304733058849</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>45</v>
       </c>
@@ -487,8 +539,27 @@
       <c r="K6">
         <v>209984.15213946099</v>
       </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M6">
+        <v>100</v>
+      </c>
+      <c r="N6">
+        <f t="shared" ref="N6:N17" si="1">(H6*(8.99/31.25)+H23*(13.42/31.25)+H40*(8.84/31.25))/5.28</f>
+        <v>102435.86363663957</v>
+      </c>
+      <c r="O6">
+        <f t="shared" si="0"/>
+        <v>185934.77694985934</v>
+      </c>
+      <c r="P6">
+        <f t="shared" si="0"/>
+        <v>49300.656554222245</v>
+      </c>
+      <c r="Q6">
+        <f t="shared" si="0"/>
+        <v>31540.412438658208</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>55</v>
       </c>
@@ -510,8 +581,27 @@
       <c r="K7">
         <v>209984.15213946099</v>
       </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M7">
+        <v>200</v>
+      </c>
+      <c r="N7">
+        <f t="shared" si="1"/>
+        <v>132123.82520055055</v>
+      </c>
+      <c r="O7">
+        <f t="shared" si="0"/>
+        <v>197704.49957957448</v>
+      </c>
+      <c r="P7">
+        <f t="shared" si="0"/>
+        <v>72517.744249423471</v>
+      </c>
+      <c r="Q7">
+        <f t="shared" si="0"/>
+        <v>33811.411563583766</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>60</v>
       </c>
@@ -533,8 +623,27 @@
       <c r="K8">
         <v>285261.48969889001</v>
       </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M8">
+        <v>300</v>
+      </c>
+      <c r="N8">
+        <f t="shared" si="1"/>
+        <v>148444.12617820938</v>
+      </c>
+      <c r="O8">
+        <f t="shared" si="0"/>
+        <v>215417.0535186429</v>
+      </c>
+      <c r="P8">
+        <f t="shared" si="0"/>
+        <v>90060.434468106891</v>
+      </c>
+      <c r="Q8">
+        <f t="shared" si="0"/>
+        <v>43156.696519503159</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>65</v>
       </c>
@@ -556,8 +665,27 @@
       <c r="K9">
         <v>360538.82725832</v>
       </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M9">
+        <v>400</v>
+      </c>
+      <c r="N9">
+        <f t="shared" si="1"/>
+        <v>161415.07981062011</v>
+      </c>
+      <c r="O9">
+        <f t="shared" si="0"/>
+        <v>236681.67840805609</v>
+      </c>
+      <c r="P9">
+        <f t="shared" si="0"/>
+        <v>102251.62431304832</v>
+      </c>
+      <c r="Q9">
+        <f t="shared" si="0"/>
+        <v>53102.474472658614</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>70</v>
       </c>
@@ -579,8 +707,27 @@
       <c r="K10">
         <v>459587.95562599</v>
       </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M10">
+        <v>500</v>
+      </c>
+      <c r="N10">
+        <f t="shared" si="1"/>
+        <v>168458.5224419091</v>
+      </c>
+      <c r="O10">
+        <f t="shared" si="0"/>
+        <v>265125.61201784608</v>
+      </c>
+      <c r="P10">
+        <f t="shared" si="0"/>
+        <v>110949.30805876748</v>
+      </c>
+      <c r="Q10">
+        <f t="shared" si="0"/>
+        <v>68093.693131891909</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>75</v>
       </c>
@@ -602,8 +749,27 @@
       <c r="K11">
         <v>495245.64183835097</v>
       </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M11">
+        <v>650</v>
+      </c>
+      <c r="N11">
+        <f t="shared" si="1"/>
+        <v>168975.10836310734</v>
+      </c>
+      <c r="O11">
+        <f t="shared" si="0"/>
+        <v>285929.63382744114</v>
+      </c>
+      <c r="P11">
+        <f t="shared" si="0"/>
+        <v>118324.31274089281</v>
+      </c>
+      <c r="Q11">
+        <f t="shared" si="0"/>
+        <v>71691.682581949673</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>85</v>
       </c>
@@ -625,8 +791,27 @@
       <c r="K12">
         <v>491283.67670364399</v>
       </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M12">
+        <v>800</v>
+      </c>
+      <c r="N12">
+        <f t="shared" si="1"/>
+        <v>170458.45620215766</v>
+      </c>
+      <c r="O12">
+        <f t="shared" si="0"/>
+        <v>297662.5575940829</v>
+      </c>
+      <c r="P12">
+        <f t="shared" si="0"/>
+        <v>121526.37978388015</v>
+      </c>
+      <c r="Q12">
+        <f t="shared" si="0"/>
+        <v>71592.455197679417</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>95</v>
       </c>
@@ -634,22 +819,41 @@
         <v>1192551.50554675</v>
       </c>
       <c r="G13">
-        <v>1500</v>
+        <v>1200</v>
       </c>
       <c r="H13">
-        <v>1224247.2266243999</v>
+        <v>1202010.9689213799</v>
       </c>
       <c r="I13">
-        <v>2218700.4754358102</v>
+        <v>2207495.4296160801</v>
       </c>
       <c r="J13">
-        <v>725039.61965134705</v>
+        <v>795246.80073126103</v>
       </c>
       <c r="K13">
-        <v>471473.85103011102</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+        <v>507312.61425959697</v>
+      </c>
+      <c r="M13">
+        <v>1200</v>
+      </c>
+      <c r="N13">
+        <f t="shared" si="1"/>
+        <v>173835.12125311076</v>
+      </c>
+      <c r="O13">
+        <f t="shared" si="0"/>
+        <v>321229.11934825976</v>
+      </c>
+      <c r="P13">
+        <f t="shared" si="0"/>
+        <v>117761.84051865866</v>
+      </c>
+      <c r="Q13">
+        <f t="shared" si="0"/>
+        <v>73373.201951748255</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>100</v>
       </c>
@@ -657,22 +861,41 @@
         <v>1196513.4706814501</v>
       </c>
       <c r="G14">
-        <v>2500</v>
+        <v>1500</v>
       </c>
       <c r="H14">
-        <v>1354992.0760697301</v>
+        <v>1224247.2266243999</v>
       </c>
       <c r="I14">
-        <v>2385103.0110935001</v>
+        <v>2218700.4754358102</v>
       </c>
       <c r="J14">
-        <v>594294.77020602196</v>
+        <v>725039.61965134705</v>
       </c>
       <c r="K14">
-        <v>431854.19968304201</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+        <v>471473.85103011102</v>
+      </c>
+      <c r="M14">
+        <v>1500</v>
+      </c>
+      <c r="N14">
+        <f t="shared" si="1"/>
+        <v>166597.27224703401</v>
+      </c>
+      <c r="O14">
+        <f t="shared" si="0"/>
+        <v>301017.62474187091</v>
+      </c>
+      <c r="P14">
+        <f t="shared" si="0"/>
+        <v>100407.00187292889</v>
+      </c>
+      <c r="Q14">
+        <f t="shared" si="0"/>
+        <v>64679.200883638237</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>120</v>
       </c>
@@ -680,22 +903,41 @@
         <v>1208399.3660855701</v>
       </c>
       <c r="G15">
-        <v>3500</v>
+        <v>2500</v>
       </c>
       <c r="H15">
-        <v>1426307.44849445</v>
+        <v>1354992.0760697301</v>
       </c>
       <c r="I15">
-        <v>2567353.4072900098</v>
+        <v>2385103.0110935001</v>
       </c>
       <c r="J15">
-        <v>530903.32805071305</v>
+        <v>594294.77020602196</v>
       </c>
       <c r="K15">
-        <v>419968.30427892198</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+        <v>431854.19968304201</v>
+      </c>
+      <c r="M15">
+        <v>2500</v>
+      </c>
+      <c r="N15">
+        <f t="shared" si="1"/>
+        <v>184032.56014983423</v>
+      </c>
+      <c r="O15">
+        <f t="shared" si="0"/>
+        <v>323618.1145848335</v>
+      </c>
+      <c r="P15">
+        <f t="shared" si="0"/>
+        <v>80071.55549152373</v>
+      </c>
+      <c r="Q15">
+        <f t="shared" si="0"/>
+        <v>58331.412380540613</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>140</v>
       </c>
@@ -703,41 +945,91 @@
         <v>1216323.29635499</v>
       </c>
       <c r="G16">
-        <v>4400</v>
+        <v>3500</v>
       </c>
       <c r="H16">
-        <v>1477812.9952456399</v>
+        <v>1426307.44849445</v>
       </c>
       <c r="I16">
-        <v>2674326.4659270998</v>
+        <v>2567353.4072900098</v>
       </c>
       <c r="J16">
-        <v>499207.60697305802</v>
+        <v>530903.32805071305</v>
       </c>
       <c r="K16">
-        <v>332805.07131537201</v>
-      </c>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+        <v>419968.30427892198</v>
+      </c>
+      <c r="M16">
+        <v>3500</v>
+      </c>
+      <c r="N16">
+        <f t="shared" si="1"/>
+        <v>193396.24453728981</v>
+      </c>
+      <c r="O16">
+        <f t="shared" si="0"/>
+        <v>349337.75152475521</v>
+      </c>
+      <c r="P16">
+        <f t="shared" si="0"/>
+        <v>72106.324737069561</v>
+      </c>
+      <c r="Q16">
+        <f t="shared" si="0"/>
+        <v>56072.612015559615</v>
+      </c>
+    </row>
+    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>160</v>
       </c>
       <c r="B17">
         <v>1220285.26148969</v>
       </c>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="G17">
+        <v>4400</v>
+      </c>
+      <c r="H17">
+        <v>1477812.9952456399</v>
+      </c>
+      <c r="I17">
+        <v>2674326.4659270998</v>
+      </c>
+      <c r="J17">
+        <v>499207.60697305802</v>
+      </c>
+      <c r="K17">
+        <v>332805.07131537201</v>
+      </c>
+      <c r="M17">
+        <v>4400</v>
+      </c>
+      <c r="N17">
+        <f t="shared" si="1"/>
+        <v>200069.39441963137</v>
+      </c>
+      <c r="O17">
+        <f t="shared" si="0"/>
+        <v>362899.91835950606</v>
+      </c>
+      <c r="P17">
+        <f t="shared" si="0"/>
+        <v>67479.229697930074</v>
+      </c>
+      <c r="Q17">
+        <f t="shared" si="0"/>
+        <v>45523.219516880323</v>
+      </c>
+    </row>
+    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>190</v>
       </c>
       <c r="B18">
         <v>1255942.94770206</v>
       </c>
-      <c r="G18" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>230</v>
       </c>
@@ -745,10 +1037,10 @@
         <v>1295562.59904912</v>
       </c>
       <c r="G19" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>270</v>
       </c>
@@ -756,33 +1048,33 @@
         <v>1354992.0760697301</v>
       </c>
       <c r="G20" t="s">
-        <v>7</v>
-      </c>
-      <c r="H20" t="s">
-        <v>8</v>
-      </c>
-      <c r="I20" t="s">
-        <v>9</v>
-      </c>
-      <c r="J20" t="s">
-        <v>6</v>
-      </c>
-      <c r="K20" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>320</v>
       </c>
       <c r="B21">
         <v>1442155.30903328</v>
       </c>
-      <c r="G21">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="G21" t="s">
+        <v>7</v>
+      </c>
+      <c r="H21" t="s">
+        <v>8</v>
+      </c>
+      <c r="I21" t="s">
+        <v>9</v>
+      </c>
+      <c r="J21" t="s">
+        <v>6</v>
+      </c>
+      <c r="K21" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>375</v>
       </c>
@@ -790,10 +1082,22 @@
         <v>1549128.36767036</v>
       </c>
       <c r="G22">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+      <c r="H22">
+        <v>324881.14104595798</v>
+      </c>
+      <c r="I22">
+        <v>966719.492868462</v>
+      </c>
+      <c r="J22">
+        <v>67353.407290015806</v>
+      </c>
+      <c r="K22">
+        <v>190174.32646592701</v>
+      </c>
+    </row>
+    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>440</v>
       </c>
@@ -801,10 +1105,22 @@
         <v>1656101.42630744</v>
       </c>
       <c r="G23">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+        <v>100</v>
+      </c>
+      <c r="H23">
+        <v>681458.00316957198</v>
+      </c>
+      <c r="I23">
+        <v>1192551.50554675</v>
+      </c>
+      <c r="J23">
+        <v>312995.245641838</v>
+      </c>
+      <c r="K23">
+        <v>206022.187004754</v>
+      </c>
+    </row>
+    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>480</v>
       </c>
@@ -812,10 +1128,22 @@
         <v>1755150.5546751099</v>
       </c>
       <c r="G24">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+        <v>200</v>
+      </c>
+      <c r="H24">
+        <v>879556.25990491197</v>
+      </c>
+      <c r="I24">
+        <v>1291600.6339144199</v>
+      </c>
+      <c r="J24">
+        <v>459587.95562599</v>
+      </c>
+      <c r="K24">
+        <v>225832.01267828801</v>
+      </c>
+    </row>
+    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>530</v>
       </c>
@@ -823,10 +1151,22 @@
         <v>1834389.8573692499</v>
       </c>
       <c r="G25">
-        <v>400</v>
-      </c>
-    </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+        <v>300</v>
+      </c>
+      <c r="H25">
+        <v>1014263.07448494</v>
+      </c>
+      <c r="I25">
+        <v>1434231.3787638601</v>
+      </c>
+      <c r="J25">
+        <v>558637.08399366005</v>
+      </c>
+      <c r="K25">
+        <v>289223.454833597</v>
+      </c>
+    </row>
+    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>625</v>
       </c>
@@ -834,10 +1174,22 @@
         <v>1921553.0903328001</v>
       </c>
       <c r="G26">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+        <v>400</v>
+      </c>
+      <c r="H26">
+        <v>1117274.1679873201</v>
+      </c>
+      <c r="I26">
+        <v>1600633.91442155</v>
+      </c>
+      <c r="J26">
+        <v>653724.24722662405</v>
+      </c>
+      <c r="K26">
+        <v>360538.82725832</v>
+      </c>
+    </row>
+    <row r="27" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>740</v>
       </c>
@@ -845,10 +1197,22 @@
         <v>1988906.4976228201</v>
       </c>
       <c r="G27">
-        <v>650</v>
-      </c>
-    </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+        <v>500</v>
+      </c>
+      <c r="H27">
+        <v>1168779.7147385101</v>
+      </c>
+      <c r="I27">
+        <v>1790808.2408874801</v>
+      </c>
+      <c r="J27">
+        <v>717115.68938193296</v>
+      </c>
+      <c r="K27">
+        <v>471473.85103011102</v>
+      </c>
+    </row>
+    <row r="28" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>900</v>
       </c>
@@ -856,10 +1220,22 @@
         <v>2080031.69572107</v>
       </c>
       <c r="G28">
-        <v>800</v>
-      </c>
-    </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+        <v>650</v>
+      </c>
+      <c r="H28">
+        <v>1176703.64500792</v>
+      </c>
+      <c r="I28">
+        <v>1941362.9160063299</v>
+      </c>
+      <c r="J28">
+        <v>768621.236133122</v>
+      </c>
+      <c r="K28">
+        <v>491283.67670364399</v>
+      </c>
+    </row>
+    <row r="29" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>1100</v>
       </c>
@@ -867,10 +1243,22 @@
         <v>2167194.9286846202</v>
       </c>
       <c r="G29">
-        <v>1500</v>
-      </c>
-    </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+        <v>800</v>
+      </c>
+      <c r="H29">
+        <v>1176703.64500792</v>
+      </c>
+      <c r="I29">
+        <v>2032488.1141045899</v>
+      </c>
+      <c r="J29">
+        <v>808240.88748019002</v>
+      </c>
+      <c r="K29">
+        <v>499207.60697305802</v>
+      </c>
+    </row>
+    <row r="30" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>1300</v>
       </c>
@@ -878,10 +1266,22 @@
         <v>2222662.4405705198</v>
       </c>
       <c r="G30">
-        <v>2500</v>
-      </c>
-    </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+        <v>1200</v>
+      </c>
+      <c r="H30">
+        <v>1180665.6101426301</v>
+      </c>
+      <c r="I30">
+        <v>2194928.6846275702</v>
+      </c>
+      <c r="J30">
+        <v>792393.026941363</v>
+      </c>
+      <c r="K30">
+        <v>519017.43264659197</v>
+      </c>
+    </row>
+    <row r="31" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>1650</v>
       </c>
@@ -889,10 +1289,22 @@
         <v>2210776.5451663998</v>
       </c>
       <c r="G31">
-        <v>3500</v>
-      </c>
-    </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+        <v>1500</v>
+      </c>
+      <c r="H31">
+        <v>1228209.19175911</v>
+      </c>
+      <c r="I31">
+        <v>2214738.5103011001</v>
+      </c>
+      <c r="J31">
+        <v>748811.410459587</v>
+      </c>
+      <c r="K31">
+        <v>479397.78129952401</v>
+      </c>
+    </row>
+    <row r="32" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>2100</v>
       </c>
@@ -900,7 +1312,19 @@
         <v>2230586.3708399301</v>
       </c>
       <c r="G32">
-        <v>4400</v>
+        <v>2500</v>
+      </c>
+      <c r="H32">
+        <v>1354992.0760697301</v>
+      </c>
+      <c r="I32">
+        <v>2381141.04595879</v>
+      </c>
+      <c r="J32">
+        <v>586370.83993660798</v>
+      </c>
+      <c r="K32">
+        <v>427892.23454833502</v>
       </c>
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.25">
@@ -910,6 +1334,21 @@
       <c r="B33">
         <v>2507923.9302694099</v>
       </c>
+      <c r="G33">
+        <v>3500</v>
+      </c>
+      <c r="H33">
+        <v>1422345.4833597401</v>
+      </c>
+      <c r="I33">
+        <v>2575277.3375594201</v>
+      </c>
+      <c r="J33">
+        <v>530903.32805071305</v>
+      </c>
+      <c r="K33">
+        <v>408082.40887480101</v>
+      </c>
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34">
@@ -918,89 +1357,214 @@
       <c r="B34">
         <v>2674326.4659270998</v>
       </c>
-      <c r="G34" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="G35" t="s">
-        <v>14</v>
+      <c r="G34">
+        <v>4400</v>
+      </c>
+      <c r="H34">
+        <v>1469889.06497622</v>
+      </c>
+      <c r="I34">
+        <v>2670364.5007923902</v>
+      </c>
+      <c r="J34">
+        <v>495245.64183835097</v>
+      </c>
+      <c r="K34">
+        <v>336767.036450079</v>
       </c>
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.25">
       <c r="G36" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="G37" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="G38" t="s">
         <v>7</v>
       </c>
-      <c r="H36" t="s">
+      <c r="H38" t="s">
         <v>8</v>
       </c>
-      <c r="I36" t="s">
+      <c r="I38" t="s">
         <v>9</v>
       </c>
-      <c r="J36" t="s">
+      <c r="J38" t="s">
         <v>6</v>
       </c>
-      <c r="K36" t="s">
+      <c r="K38" t="s">
         <v>10</v>
-      </c>
-    </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="G37">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="G38">
-        <v>100</v>
       </c>
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.25">
       <c r="G39">
-        <v>200</v>
+        <v>15</v>
+      </c>
+      <c r="H39">
+        <v>111658.45648604201</v>
+      </c>
+      <c r="I39">
+        <v>547619.04761904699</v>
+      </c>
+      <c r="J39">
+        <v>32840.722495894901</v>
+      </c>
+      <c r="K39">
+        <v>104269.29392446599</v>
       </c>
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.25">
       <c r="G40">
-        <v>300</v>
+        <v>100</v>
+      </c>
+      <c r="H40">
+        <v>212643.67816091899</v>
+      </c>
+      <c r="I40">
+        <v>439244.66338259401</v>
+      </c>
+      <c r="J40">
+        <v>142857.142857142</v>
+      </c>
+      <c r="K40">
+        <v>62397.372742200299</v>
       </c>
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.25">
       <c r="G41">
-        <v>400</v>
+        <v>200</v>
+      </c>
+      <c r="H41">
+        <v>232348.11165845601</v>
+      </c>
+      <c r="I41">
+        <v>440065.68144499097</v>
+      </c>
+      <c r="J41">
+        <v>212643.67816091899</v>
+      </c>
+      <c r="K41">
+        <v>74712.643678160894</v>
       </c>
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.25">
       <c r="G42">
-        <v>500</v>
+        <v>300</v>
+      </c>
+      <c r="H42">
+        <v>199507.38916256101</v>
+      </c>
+      <c r="I42">
+        <v>421182.266009852</v>
+      </c>
+      <c r="J42">
+        <v>244663.38259441699</v>
+      </c>
+      <c r="K42">
+        <v>76354.679802955696</v>
       </c>
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.25">
       <c r="G43">
-        <v>650</v>
+        <v>400</v>
+      </c>
+      <c r="H43">
+        <v>172413.793103448</v>
+      </c>
+      <c r="I43">
+        <v>380131.36288998299</v>
+      </c>
+      <c r="J43">
+        <v>255336.61740558199</v>
+      </c>
+      <c r="K43">
+        <v>77175.697865352995</v>
       </c>
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.25">
       <c r="G44">
-        <v>800</v>
+        <v>500</v>
+      </c>
+      <c r="H44">
+        <v>177339.901477832</v>
+      </c>
+      <c r="I44">
+        <v>404761.90476190398</v>
+      </c>
+      <c r="J44">
+        <v>256978.65353037699</v>
+      </c>
+      <c r="K44">
+        <v>87848.932676518903</v>
       </c>
     </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.25">
       <c r="G45">
-        <v>1500</v>
+        <v>650</v>
+      </c>
+      <c r="H45">
+        <v>178981.937602627</v>
+      </c>
+      <c r="I45">
+        <v>415435.13957306999</v>
+      </c>
+      <c r="J45">
+        <v>247947.45484400599</v>
+      </c>
+      <c r="K45">
+        <v>88669.950738916305</v>
       </c>
     </row>
     <row r="46" spans="1:11" x14ac:dyDescent="0.25">
       <c r="G46">
-        <v>2500</v>
+        <v>800</v>
+      </c>
+      <c r="H46">
+        <v>194581.28078817701</v>
+      </c>
+      <c r="I46">
+        <v>419540.22988505702</v>
+      </c>
+      <c r="J46">
+        <v>227422.00328407201</v>
+      </c>
+      <c r="K46">
+        <v>78817.733990147797</v>
       </c>
     </row>
     <row r="47" spans="1:11" x14ac:dyDescent="0.25">
       <c r="G47">
-        <v>3500</v>
+        <v>1200</v>
+      </c>
+      <c r="H47">
+        <v>229885.05747126401</v>
+      </c>
+      <c r="I47">
+        <v>418719.21182266</v>
+      </c>
+      <c r="J47">
+        <v>186371.100164203</v>
+      </c>
+      <c r="K47">
+        <v>65681.444991789802</v>
       </c>
     </row>
     <row r="48" spans="1:11" x14ac:dyDescent="0.25">
       <c r="G48">
+        <v>2500</v>
+      </c>
+    </row>
+    <row r="49" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G49">
+        <v>3500</v>
+      </c>
+    </row>
+    <row r="50" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G50">
         <v>4400</v>
       </c>
     </row>

</xml_diff>